<commit_message>
ascii progress bar - done
</commit_message>
<xml_diff>
--- a/links.xlsx
+++ b/links.xlsx
@@ -25,55 +25,55 @@
     <t>00-01051533</t>
   </si>
   <si>
-    <t>http://new.nnz-ipc.ru//catalogue/komp_yutery_i_komplektuyuwie/passivnye_kross-platy/isa/bp-14sd/</t>
+    <t>BP-14SD</t>
   </si>
   <si>
     <t>00-01051535</t>
   </si>
   <si>
-    <t>http://new.nnz-ipc.ru//catalogue/komp_yutery_i_komplektuyuwie/passivnye_kross-platy/isa/bp-20sd/</t>
+    <t>BP-20SD</t>
   </si>
   <si>
     <t>00-01059304</t>
   </si>
   <si>
-    <t>http://new.nnz-ipc.ru//catalogue/komp_yutery_i_komplektuyuwie/passivnye_kross-platy/picmg_1_0/pci-19s/</t>
+    <t>PCI-19S</t>
   </si>
   <si>
     <t>00-01062148</t>
   </si>
   <si>
-    <t>http://new.nnz-ipc.ru//catalogue/komp_yutery_i_komplektuyuwie/passivnye_kross-platy/isa/bp-10sd/</t>
+    <t>BP-10SD</t>
   </si>
   <si>
     <t>00-01075733</t>
   </si>
   <si>
-    <t>http://new.nnz-ipc.ru//catalogue/komp_yutery_i_komplektuyuwie/passivnye_kross-platy/picmg_1_0/pci-17sq/</t>
+    <t>PCI-17SQ</t>
   </si>
   <si>
     <t>00-01075734</t>
   </si>
   <si>
-    <t>http://new.nnz-ipc.ru//catalogue/komp_yutery_i_komplektuyuwie/passivnye_kross-platy/picmg_1_0/px-8s/</t>
+    <t>PX-8S</t>
   </si>
   <si>
     <t>00-01131268</t>
   </si>
   <si>
-    <t>http://new.nnz-ipc.ru//catalogue/komp_yutery_i_komplektuyuwie/passivnye_kross-platy/pcisa/ip-4sa/</t>
+    <t>IP-4SA</t>
   </si>
   <si>
     <t>00-01179217</t>
   </si>
   <si>
-    <t>http://new.nnz-ipc.ru//catalogue/komp_yutery_i_komplektuyuwie/passivnye_kross-platy/picmg_1_3/pxe-19s/</t>
+    <t>PXE-19S</t>
   </si>
   <si>
     <t>00-05000548</t>
   </si>
   <si>
-    <t>http://new.nnz-ipc.ru//catalogue/komp_yutery_i_komplektuyuwie/passivnye_kross-platy/picmg_1_0/px-20s3/</t>
+    <t>PX-20S3</t>
   </si>
 </sst>
 </file>
@@ -214,5 +214,16 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+  </hyperlinks>
 </worksheet>
 </file>
</xml_diff>